<commit_message>
nueva version GTFS 2019-10-12
</commit_message>
<xml_diff>
--- a/inputs/bip/bip_center_high_level.xlsx
+++ b/inputs/bip/bip_center_high_level.xlsx
@@ -1000,11 +1000,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:O44"/>
+  <dimension ref="B3:T44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:B44"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1135,7 +1133,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="12" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B17" s="10">
         <v>3</v>
       </c>
@@ -1164,7 +1162,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="2:15" ht="12" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B18" s="10">
         <v>4</v>
       </c>
@@ -1193,7 +1191,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="2:15" ht="12" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B19" s="10">
         <v>6</v>
       </c>
@@ -1222,7 +1220,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="2:15" ht="12" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B20" s="10">
         <v>7</v>
       </c>
@@ -1251,7 +1249,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="2:15" ht="12" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B21" s="10">
         <v>9</v>
       </c>
@@ -1280,7 +1278,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="2:15" ht="12" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B22" s="10">
         <v>12</v>
       </c>
@@ -1309,7 +1307,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="2:15" ht="12" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B23" s="10">
         <v>13</v>
       </c>
@@ -1338,7 +1336,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="2:15" ht="12" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B24" s="10">
         <v>15</v>
       </c>
@@ -1367,7 +1365,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="2:15" ht="12" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B25" s="10">
         <v>24</v>
       </c>
@@ -1396,7 +1394,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="2:15" ht="12" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B26" s="10">
         <v>26</v>
       </c>
@@ -1425,7 +1423,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="2:15" ht="12" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B27" s="10">
         <v>34</v>
       </c>
@@ -1454,7 +1452,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="2:15" ht="12" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B28" s="10">
         <v>36</v>
       </c>
@@ -1483,7 +1481,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="2:15" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:20" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="B29" s="13">
         <v>41</v>
       </c>
@@ -1516,8 +1514,13 @@
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
-    </row>
-    <row r="30" spans="2:15" ht="12" x14ac:dyDescent="0.2">
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+    </row>
+    <row r="30" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B30" s="10">
         <v>44</v>
       </c>
@@ -1546,7 +1549,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="2:15" ht="12" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B31" s="10">
         <v>49</v>
       </c>
@@ -1575,7 +1578,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="2:15" ht="12" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B32" s="10">
         <v>55</v>
       </c>
@@ -1604,7 +1607,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="2:15" ht="12" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B33" s="10">
         <v>59</v>
       </c>
@@ -1633,7 +1636,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="2:15" ht="12" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B34" s="10">
         <v>64</v>
       </c>
@@ -1662,7 +1665,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="2:15" ht="12" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B35" s="10">
         <v>66</v>
       </c>
@@ -1691,7 +1694,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="2:15" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:20" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="B36" s="13">
         <v>71</v>
       </c>
@@ -1724,8 +1727,13 @@
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
-    </row>
-    <row r="37" spans="2:15" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+    </row>
+    <row r="37" spans="2:20" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="B37" s="13">
         <v>78</v>
       </c>
@@ -1758,8 +1766,13 @@
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
-    </row>
-    <row r="38" spans="2:15" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+    </row>
+    <row r="38" spans="2:20" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="B38" s="13">
         <v>79</v>
       </c>
@@ -1792,8 +1805,13 @@
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
-    </row>
-    <row r="39" spans="2:15" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+    </row>
+    <row r="39" spans="2:20" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="B39" s="13">
         <v>90</v>
       </c>
@@ -1826,8 +1844,13 @@
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
-    </row>
-    <row r="40" spans="2:15" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+    </row>
+    <row r="40" spans="2:20" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="B40" s="13">
         <v>93</v>
       </c>
@@ -1860,8 +1883,13 @@
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
-    </row>
-    <row r="41" spans="2:15" ht="12" x14ac:dyDescent="0.2">
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+    </row>
+    <row r="41" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B41" s="10">
         <v>95</v>
       </c>
@@ -1890,7 +1918,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="2:15" ht="12" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B42" s="10">
         <v>98</v>
       </c>
@@ -1919,7 +1947,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="43" spans="2:15" ht="12" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B43" s="10">
         <v>113</v>
       </c>
@@ -1948,7 +1976,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="2:15" ht="12" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B44" s="10">
         <v>115</v>
       </c>

</xml_diff>

<commit_message>
version de 2020-01-11 + actualizacion bip
</commit_message>
<xml_diff>
--- a/inputs/bip/bip_center_high_level.xlsx
+++ b/inputs/bip/bip_center_high_level.xlsx
@@ -7,17 +7,18 @@
     <workbookView xWindow="240" yWindow="495" windowWidth="15480" windowHeight="7710" tabRatio="713"/>
   </bookViews>
   <sheets>
-    <sheet name="PCMAV ALTO ESTANDAR" sheetId="1" r:id="rId1"/>
+    <sheet name="Abiertos" sheetId="1" r:id="rId1"/>
+    <sheet name="Cerrados" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PCMAV ALTO ESTANDAR'!$B$15:$J$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Abiertos!$B$15:$J$34</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="133">
   <si>
     <t>CODIGO</t>
   </si>
@@ -1000,7 +1001,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:T44"/>
+  <dimension ref="B3:T38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -1106,902 +1107,718 @@
     </row>
     <row r="16" spans="2:10" ht="12" x14ac:dyDescent="0.2">
       <c r="B16" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>46</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>115</v>
       </c>
       <c r="G16" s="9">
-        <v>339123</v>
+        <v>352564</v>
       </c>
       <c r="H16" s="9">
-        <v>6306982</v>
+        <v>6286262</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B17" s="10">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>46</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>115</v>
       </c>
       <c r="G17" s="9">
-        <v>352564</v>
+        <v>347803</v>
       </c>
       <c r="H17" s="9">
-        <v>6286262</v>
+        <v>6306036</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B18" s="10">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>46</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>115</v>
       </c>
       <c r="G18" s="9">
-        <v>347803</v>
+        <v>343185</v>
       </c>
       <c r="H18" s="9">
-        <v>6306036</v>
+        <v>6306004</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B19" s="10">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>46</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>115</v>
       </c>
       <c r="G19" s="9">
-        <v>347803</v>
+        <v>351432</v>
       </c>
       <c r="H19" s="9">
-        <v>6306036</v>
+        <v>6293259</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B20" s="10">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>46</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>115</v>
       </c>
       <c r="G20" s="9">
-        <v>348592</v>
+        <v>341609</v>
       </c>
       <c r="H20" s="9">
-        <v>6286067</v>
+        <v>6302502</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B21" s="10">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="G21" s="9">
-        <v>343185</v>
+        <v>355739</v>
       </c>
       <c r="H21" s="9">
-        <v>6306004</v>
+        <v>6300507</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B22" s="10">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>46</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>115</v>
       </c>
       <c r="G22" s="9">
-        <v>351432</v>
+        <v>347788</v>
       </c>
       <c r="H22" s="9">
-        <v>6293259</v>
+        <v>6291309</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B23" s="10">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>46</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>115</v>
       </c>
       <c r="G23" s="9">
-        <v>342431</v>
+        <v>337199</v>
       </c>
       <c r="H23" s="9">
-        <v>6289583</v>
+        <v>6298107</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B24" s="10">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="G24" s="9">
-        <v>341609</v>
+        <v>350549</v>
       </c>
       <c r="H24" s="9">
-        <v>6302502</v>
+        <v>6298998</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="2:20" ht="12" x14ac:dyDescent="0.2">
-      <c r="B25" s="10">
-        <v>24</v>
-      </c>
-      <c r="C25" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="2:20" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="B25" s="13">
+        <v>41</v>
+      </c>
+      <c r="C25" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F25" s="9" t="s">
+      <c r="D25" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="G25" s="9">
-        <v>355739</v>
-      </c>
-      <c r="H25" s="9">
-        <v>6300507</v>
-      </c>
-      <c r="I25" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="J25" s="9" t="s">
-        <v>86</v>
-      </c>
+      <c r="G25" s="15">
+        <v>341989</v>
+      </c>
+      <c r="H25" s="15">
+        <v>6281837</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="J25" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
     </row>
     <row r="26" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B26" s="10">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>46</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>115</v>
       </c>
       <c r="G26" s="9">
-        <v>347788</v>
+        <v>340246</v>
       </c>
       <c r="H26" s="9">
-        <v>6291309</v>
+        <v>6299652</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B27" s="10">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>22</v>
+        <v>119</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>115</v>
       </c>
       <c r="G27" s="9">
-        <v>337199</v>
+        <v>347137</v>
       </c>
       <c r="H27" s="9">
-        <v>6298107</v>
+        <v>6296695</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B28" s="10">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="G28" s="9">
-        <v>350549</v>
+        <v>341522</v>
       </c>
       <c r="H28" s="9">
-        <v>6298998</v>
+        <v>6295906</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="2:20" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="B29" s="13">
-        <v>41</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="G29" s="15">
-        <v>341989</v>
-      </c>
-      <c r="H29" s="15">
-        <v>6281837</v>
-      </c>
-      <c r="I29" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="J29" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
-      <c r="R29" s="2"/>
-      <c r="S29" s="2"/>
-      <c r="T29" s="2"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20" ht="12" x14ac:dyDescent="0.2">
+      <c r="B29" s="10">
+        <v>64</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G29" s="9">
+        <v>348432</v>
+      </c>
+      <c r="H29" s="9">
+        <v>6302977</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="J29" s="9" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="30" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B30" s="10">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>115</v>
       </c>
       <c r="G30" s="9">
-        <v>338267</v>
+        <v>345636</v>
       </c>
       <c r="H30" s="9">
-        <v>6294537</v>
+        <v>6302389</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="2:20" ht="12" x14ac:dyDescent="0.2">
-      <c r="B31" s="10">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="B31" s="13">
+        <v>71</v>
+      </c>
+      <c r="C31" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="G31" s="9">
-        <v>340246</v>
-      </c>
-      <c r="H31" s="9">
-        <v>6299652</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="J31" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="2:20" ht="12" x14ac:dyDescent="0.2">
-      <c r="B32" s="10">
-        <v>55</v>
-      </c>
-      <c r="C32" s="11" t="s">
+      <c r="D31" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="G31" s="15">
+        <v>340044</v>
+      </c>
+      <c r="H31" s="15">
+        <v>6292857</v>
+      </c>
+      <c r="I31" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="J31" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+    </row>
+    <row r="32" spans="2:20" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="B32" s="13">
+        <v>78</v>
+      </c>
+      <c r="C32" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="E32" s="12" t="s">
+      <c r="D32" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="G32" s="15">
+        <v>344292</v>
+      </c>
+      <c r="H32" s="15">
+        <v>6292613</v>
+      </c>
+      <c r="I32" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="J32" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+    </row>
+    <row r="33" spans="2:20" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="B33" s="13">
+        <v>79</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F32" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="G32" s="9">
-        <v>347137</v>
-      </c>
-      <c r="H32" s="9">
-        <v>6296695</v>
-      </c>
-      <c r="I32" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="J32" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="33" spans="2:20" ht="12" x14ac:dyDescent="0.2">
-      <c r="B33" s="10">
-        <v>59</v>
-      </c>
-      <c r="C33" s="11" t="s">
+      <c r="F33" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="G33" s="15">
+        <v>347030</v>
+      </c>
+      <c r="H33" s="15">
+        <v>6297244</v>
+      </c>
+      <c r="I33" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="J33" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+    </row>
+    <row r="34" spans="2:20" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="B34" s="13">
+        <v>90</v>
+      </c>
+      <c r="C34" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="G33" s="9">
-        <v>341522</v>
-      </c>
-      <c r="H33" s="9">
-        <v>6295906</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="J33" s="9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="2:20" ht="12" x14ac:dyDescent="0.2">
-      <c r="B34" s="10">
-        <v>64</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="G34" s="9">
-        <v>348432</v>
-      </c>
-      <c r="H34" s="9">
-        <v>6302977</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="J34" s="9" t="s">
-        <v>102</v>
-      </c>
+      <c r="D34" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="G34" s="15">
+        <v>342600</v>
+      </c>
+      <c r="H34" s="15">
+        <v>6293992</v>
+      </c>
+      <c r="I34" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="J34" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
     </row>
     <row r="35" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B35" s="10">
-        <v>66</v>
+        <v>95</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>49</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>115</v>
       </c>
       <c r="G35" s="9">
-        <v>345636</v>
+        <v>350933</v>
       </c>
       <c r="H35" s="9">
-        <v>6302389</v>
+        <v>6296934</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="J35" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="2:20" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="B36" s="13">
-        <v>71</v>
-      </c>
-      <c r="C36" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="2:20" ht="12" x14ac:dyDescent="0.2">
+      <c r="B36" s="10">
+        <v>98</v>
+      </c>
+      <c r="C36" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="F36" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="G36" s="15">
-        <v>340044</v>
-      </c>
-      <c r="H36" s="15">
-        <v>6292857</v>
-      </c>
-      <c r="I36" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="J36" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
-      <c r="Q36" s="2"/>
-      <c r="R36" s="2"/>
-      <c r="S36" s="2"/>
-      <c r="T36" s="2"/>
-    </row>
-    <row r="37" spans="2:20" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="B37" s="13">
-        <v>78</v>
-      </c>
-      <c r="C37" s="14" t="s">
+      <c r="D36" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G36" s="9">
+        <v>356883</v>
+      </c>
+      <c r="H36" s="9">
+        <v>6297649</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="J36" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="2:20" ht="12" x14ac:dyDescent="0.2">
+      <c r="B37" s="10">
+        <v>113</v>
+      </c>
+      <c r="C37" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D37" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>63</v>
+      <c r="D37" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="F37" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="G37" s="15">
-        <v>344292</v>
-      </c>
-      <c r="H37" s="15">
-        <v>6292613</v>
-      </c>
-      <c r="I37" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="J37" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
-      <c r="P37" s="2"/>
-      <c r="Q37" s="2"/>
-      <c r="R37" s="2"/>
-      <c r="S37" s="2"/>
-      <c r="T37" s="2"/>
-    </row>
-    <row r="38" spans="2:20" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="B38" s="13">
-        <v>79</v>
-      </c>
-      <c r="C38" s="14" t="s">
+      <c r="G37" s="9">
+        <v>351539</v>
+      </c>
+      <c r="H37" s="9">
+        <v>6296091</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="J37" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="2:20" ht="12" x14ac:dyDescent="0.2">
+      <c r="B38" s="10">
+        <v>115</v>
+      </c>
+      <c r="C38" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D38" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F38" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="G38" s="15">
-        <v>347030</v>
-      </c>
-      <c r="H38" s="15">
-        <v>6297244</v>
-      </c>
-      <c r="I38" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="J38" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
-      <c r="O38" s="2"/>
-      <c r="P38" s="2"/>
-      <c r="Q38" s="2"/>
-      <c r="R38" s="2"/>
-      <c r="S38" s="2"/>
-      <c r="T38" s="2"/>
-    </row>
-    <row r="39" spans="2:20" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="B39" s="13">
-        <v>90</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="F39" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="G39" s="15">
-        <v>342600</v>
-      </c>
-      <c r="H39" s="15">
-        <v>6293992</v>
-      </c>
-      <c r="I39" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="J39" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-      <c r="Q39" s="2"/>
-      <c r="R39" s="2"/>
-      <c r="S39" s="2"/>
-      <c r="T39" s="2"/>
-    </row>
-    <row r="40" spans="2:20" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="B40" s="13">
-        <v>93</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E40" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="G40" s="15">
-        <v>336593</v>
-      </c>
-      <c r="H40" s="15">
-        <v>6290794</v>
-      </c>
-      <c r="I40" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="J40" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
-      <c r="P40" s="2"/>
-      <c r="Q40" s="2"/>
-      <c r="R40" s="2"/>
-      <c r="S40" s="2"/>
-      <c r="T40" s="2"/>
-    </row>
-    <row r="41" spans="2:20" ht="12" x14ac:dyDescent="0.2">
-      <c r="B41" s="10">
-        <v>95</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="G41" s="9">
-        <v>350933</v>
-      </c>
-      <c r="H41" s="9">
-        <v>6296934</v>
-      </c>
-      <c r="I41" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="J41" s="9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="42" spans="2:20" ht="12" x14ac:dyDescent="0.2">
-      <c r="B42" s="10">
-        <v>98</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="G42" s="9">
-        <v>356883</v>
-      </c>
-      <c r="H42" s="9">
-        <v>6297649</v>
-      </c>
-      <c r="I42" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="J42" s="9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="43" spans="2:20" ht="12" x14ac:dyDescent="0.2">
-      <c r="B43" s="10">
-        <v>113</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="E43" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F43" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="G43" s="9">
-        <v>351539</v>
-      </c>
-      <c r="H43" s="9">
-        <v>6296091</v>
-      </c>
-      <c r="I43" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="J43" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="44" spans="2:20" ht="12" x14ac:dyDescent="0.2">
-      <c r="B44" s="10">
-        <v>115</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D44" s="9" t="s">
+      <c r="D38" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E38" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F44" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="G44" s="9">
+      <c r="F38" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G38" s="9">
         <v>347885</v>
       </c>
-      <c r="H44" s="9">
+      <c r="H38" s="9">
         <v>6299307</v>
       </c>
-      <c r="I44" s="9" t="s">
+      <c r="I38" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="J44" s="9" t="s">
+      <c r="J38" s="9" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2014,4 +1831,293 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:J21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="55.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="11" style="5" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="B3" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+    </row>
+    <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B5" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="2:10" ht="12" x14ac:dyDescent="0.2">
+      <c r="B6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="2:10" ht="12" x14ac:dyDescent="0.2">
+      <c r="B7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="2:10" ht="12" x14ac:dyDescent="0.2">
+      <c r="B8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="2:10" ht="12" x14ac:dyDescent="0.2">
+      <c r="B9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="2:10" ht="12" x14ac:dyDescent="0.2">
+      <c r="B10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="2:10" ht="12" x14ac:dyDescent="0.2">
+      <c r="B11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="12" x14ac:dyDescent="0.2">
+      <c r="B16" s="10">
+        <v>2</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G16" s="9">
+        <v>339123</v>
+      </c>
+      <c r="H16" s="9">
+        <v>6306982</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="B17" s="13">
+        <v>4</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="G17" s="15">
+        <v>347803</v>
+      </c>
+      <c r="H17" s="15">
+        <v>6306036</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="12" x14ac:dyDescent="0.2">
+      <c r="B18" s="10">
+        <v>7</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G18" s="9">
+        <v>348592</v>
+      </c>
+      <c r="H18" s="9">
+        <v>6286067</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="B19" s="13">
+        <v>13</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="G19" s="15">
+        <v>342431</v>
+      </c>
+      <c r="H19" s="15">
+        <v>6289583</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="B20" s="13">
+        <v>44</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="G20" s="15">
+        <v>338267</v>
+      </c>
+      <c r="H20" s="15">
+        <v>6294537</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="B21" s="13">
+        <v>93</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="G21" s="15">
+        <v>336593</v>
+      </c>
+      <c r="H21" s="15">
+        <v>6290794</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ultima version de bip 2020-07-15
</commit_message>
<xml_diff>
--- a/inputs/bip/bip_center_high_level.xlsx
+++ b/inputs/bip/bip_center_high_level.xlsx
@@ -368,15 +368,6 @@
     <t>Lun a Vie 07:00 a 22:00 Sab 08:00 a 22:00 Dom y Festivos 09:00 a 22:00</t>
   </si>
   <si>
-    <t>BELLAVISTA FRENTE AL N° 24-36</t>
-  </si>
-  <si>
-    <t>-70.636347</t>
-  </si>
-  <si>
-    <t>-33.434846</t>
-  </si>
-  <si>
     <t>SAN FRANCISCO 1085</t>
   </si>
   <si>
@@ -417,6 +408,15 @@
   </si>
   <si>
     <t>-33.464353</t>
+  </si>
+  <si>
+    <t>CONSTITUCION 2</t>
+  </si>
+  <si>
+    <t>-70.634510</t>
+  </si>
+  <si>
+    <t>-33.434457</t>
   </si>
 </sst>
 </file>
@@ -573,7 +573,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -618,6 +618,12 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1001,7 +1007,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:T38"/>
+  <dimension ref="B3:T39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -1021,17 +1027,17 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:10" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="19"/>
+      <c r="C5" s="21"/>
       <c r="D5" s="6"/>
     </row>
     <row r="6" spans="2:10" ht="12" x14ac:dyDescent="0.2">
@@ -1109,13 +1115,13 @@
       <c r="B16" s="10">
         <v>3</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="18" t="s">
         <v>46</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="11" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="9" t="s">
@@ -1138,13 +1144,13 @@
       <c r="B17" s="10">
         <v>6</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="18" t="s">
         <v>46</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="11" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="9" t="s">
@@ -1167,13 +1173,13 @@
       <c r="B18" s="10">
         <v>9</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="18" t="s">
         <v>46</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="11" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="9" t="s">
@@ -1196,13 +1202,13 @@
       <c r="B19" s="10">
         <v>12</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="18" t="s">
         <v>46</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="11" t="s">
         <v>15</v>
       </c>
       <c r="F19" s="9" t="s">
@@ -1225,13 +1231,13 @@
       <c r="B20" s="10">
         <v>15</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="18" t="s">
         <v>46</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="11" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="9" t="s">
@@ -1254,17 +1260,17 @@
       <c r="B21" s="10">
         <v>24</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="18" t="s">
         <v>62</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="11" t="s">
         <v>57</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G21" s="9">
         <v>355739</v>
@@ -1283,13 +1289,13 @@
       <c r="B22" s="10">
         <v>26</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="18" t="s">
         <v>46</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="11" t="s">
         <v>20</v>
       </c>
       <c r="F22" s="9" t="s">
@@ -1312,13 +1318,13 @@
       <c r="B23" s="10">
         <v>34</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="18" t="s">
         <v>46</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="11" t="s">
         <v>27</v>
       </c>
       <c r="F23" s="9" t="s">
@@ -1341,17 +1347,17 @@
       <c r="B24" s="10">
         <v>36</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="18" t="s">
         <v>62</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="11" t="s">
         <v>5</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G24" s="9">
         <v>350549</v>
@@ -1367,31 +1373,31 @@
       </c>
     </row>
     <row r="25" spans="2:20" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="B25" s="13">
+      <c r="B25" s="10">
         <v>41</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F25" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="G25" s="15">
+      <c r="F25" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G25" s="9">
         <v>341989</v>
       </c>
-      <c r="H25" s="15">
+      <c r="H25" s="9">
         <v>6281837</v>
       </c>
-      <c r="I25" s="15" t="s">
+      <c r="I25" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="J25" s="15" t="s">
+      <c r="J25" s="9" t="s">
         <v>94</v>
       </c>
       <c r="K25" s="2"/>
@@ -1409,13 +1415,13 @@
       <c r="B26" s="10">
         <v>49</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="18" t="s">
         <v>46</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="11" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="9" t="s">
@@ -1438,13 +1444,13 @@
       <c r="B27" s="10">
         <v>55</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="18" t="s">
         <v>49</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="E27" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="11" t="s">
         <v>25</v>
       </c>
       <c r="F27" s="9" t="s">
@@ -1457,23 +1463,23 @@
         <v>6296695</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B28" s="10">
         <v>59</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="18" t="s">
         <v>49</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="11" t="s">
         <v>26</v>
       </c>
       <c r="F28" s="9" t="s">
@@ -1496,13 +1502,13 @@
       <c r="B29" s="10">
         <v>64</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="18" t="s">
         <v>49</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F29" s="9" t="s">
@@ -1525,13 +1531,13 @@
       <c r="B30" s="10">
         <v>66</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="18" t="s">
         <v>49</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="11" t="s">
         <v>30</v>
       </c>
       <c r="F30" s="9" t="s">
@@ -1551,32 +1557,32 @@
       </c>
     </row>
     <row r="31" spans="2:20" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="B31" s="13">
+      <c r="B31" s="10">
         <v>71</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="19" t="s">
         <v>49</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>121</v>
+        <v>124</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>118</v>
       </c>
       <c r="F31" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="G31" s="15">
+      <c r="G31" s="9">
         <v>340044</v>
       </c>
-      <c r="H31" s="15">
+      <c r="H31" s="9">
         <v>6292857</v>
       </c>
-      <c r="I31" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="J31" s="15" t="s">
-        <v>129</v>
+      <c r="I31" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="J31" s="9" t="s">
+        <v>126</v>
       </c>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
@@ -1590,31 +1596,31 @@
       <c r="T31" s="2"/>
     </row>
     <row r="32" spans="2:20" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="B32" s="13">
+      <c r="B32" s="10">
         <v>78</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="16" t="s">
+      <c r="E32" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F32" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="G32" s="15">
+      <c r="F32" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G32" s="9">
         <v>344292</v>
       </c>
-      <c r="H32" s="15">
+      <c r="H32" s="9">
         <v>6292613</v>
       </c>
-      <c r="I32" s="15" t="s">
+      <c r="I32" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="J32" s="15" t="s">
+      <c r="J32" s="9" t="s">
         <v>106</v>
       </c>
       <c r="K32" s="2"/>
@@ -1629,31 +1635,31 @@
       <c r="T32" s="2"/>
     </row>
     <row r="33" spans="2:20" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="B33" s="13">
+      <c r="B33" s="10">
         <v>79</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E33" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F33" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="G33" s="15">
+      <c r="F33" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G33" s="9">
         <v>347030</v>
       </c>
-      <c r="H33" s="15">
+      <c r="H33" s="9">
         <v>6297244</v>
       </c>
-      <c r="I33" s="15" t="s">
+      <c r="I33" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="J33" s="15" t="s">
+      <c r="J33" s="9" t="s">
         <v>108</v>
       </c>
       <c r="K33" s="2"/>
@@ -1668,32 +1674,32 @@
       <c r="T33" s="2"/>
     </row>
     <row r="34" spans="2:20" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="B34" s="13">
+      <c r="B34" s="10">
         <v>90</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="F34" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="G34" s="15">
+      <c r="D34" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G34" s="9">
         <v>342600</v>
       </c>
-      <c r="H34" s="15">
+      <c r="H34" s="9">
         <v>6293992</v>
       </c>
-      <c r="I34" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="J34" s="15" t="s">
-        <v>126</v>
+      <c r="I34" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>123</v>
       </c>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
@@ -1708,118 +1714,147 @@
     </row>
     <row r="35" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B35" s="10">
+        <v>93</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="G35" s="9">
+        <v>336593</v>
+      </c>
+      <c r="H35" s="9">
+        <v>6290794</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="J35" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="2:20" ht="12" x14ac:dyDescent="0.2">
+      <c r="B36" s="13">
         <v>95</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C36" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D36" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E36" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="F35" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="G35" s="9">
+      <c r="F36" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G36" s="9">
         <v>350933</v>
       </c>
-      <c r="H35" s="9">
+      <c r="H36" s="9">
         <v>6296934</v>
       </c>
-      <c r="I35" s="9" t="s">
+      <c r="I36" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="J35" s="9" t="s">
+      <c r="J36" s="9" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="36" spans="2:20" ht="12" x14ac:dyDescent="0.2">
-      <c r="B36" s="10">
-        <v>98</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="G36" s="9">
-        <v>356883</v>
-      </c>
-      <c r="H36" s="9">
-        <v>6297649</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="J36" s="9" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="37" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B37" s="10">
+        <v>98</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G37" s="9">
+        <v>356883</v>
+      </c>
+      <c r="H37" s="9">
+        <v>6297649</v>
+      </c>
+      <c r="I37" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C37" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F37" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="G37" s="9">
-        <v>351539</v>
-      </c>
-      <c r="H37" s="9">
-        <v>6296091</v>
-      </c>
-      <c r="I37" s="9" t="s">
-        <v>131</v>
-      </c>
       <c r="J37" s="9" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="2:20" ht="12" x14ac:dyDescent="0.2">
       <c r="B38" s="10">
-        <v>115</v>
-      </c>
-      <c r="C38" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" s="18" t="s">
         <v>49</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>29</v>
+        <v>127</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="F38" s="9" t="s">
         <v>115</v>
       </c>
       <c r="G38" s="9">
-        <v>347885</v>
+        <v>351539</v>
       </c>
       <c r="H38" s="9">
-        <v>6299307</v>
+        <v>6296091</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="J38" s="9" t="s">
-        <v>118</v>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="2:20" ht="12" x14ac:dyDescent="0.2">
+      <c r="B39" s="10">
+        <v>115</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G39" s="9">
+        <v>348055</v>
+      </c>
+      <c r="H39" s="9">
+        <v>6299353</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="J39" s="9" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1835,7 +1870,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:J21"/>
+  <dimension ref="B3:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1855,17 +1890,17 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:10" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="19"/>
+      <c r="C5" s="21"/>
       <c r="D5" s="6"/>
     </row>
     <row r="6" spans="2:10" ht="12" x14ac:dyDescent="0.2">
@@ -2082,35 +2117,6 @@
       </c>
       <c r="J20" s="15" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="B21" s="13">
-        <v>93</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="G21" s="15">
-        <v>336593</v>
-      </c>
-      <c r="H21" s="15">
-        <v>6290794</v>
-      </c>
-      <c r="I21" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="J21" s="15" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nueva version GTFS 2020-09-26
</commit_message>
<xml_diff>
--- a/inputs/bip/bip_center_high_level.xlsx
+++ b/inputs/bip/bip_center_high_level.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Cerrados" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Abiertos!$A$14:$I$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Abiertos!$A$14:$I$34</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="117">
   <si>
     <t>CODIGO</t>
   </si>
@@ -188,27 +188,6 @@
     <t>ALCALDE FERNANDO CASTILLO VELASCO 8900</t>
   </si>
   <si>
-    <t>AV. FLORENCIO BARRIOS 1660</t>
-  </si>
-  <si>
-    <t>LAS CONDES</t>
-  </si>
-  <si>
-    <t>AV. FRANCISCO BILBAO 1966</t>
-  </si>
-  <si>
-    <t>FREIRE 399</t>
-  </si>
-  <si>
-    <t>SAN BERNARDO</t>
-  </si>
-  <si>
-    <t>MANUEL RODRIGUEZ 1853</t>
-  </si>
-  <si>
-    <t>ServiEstado</t>
-  </si>
-  <si>
     <t>PEDRO AGUIRRE CERDA</t>
   </si>
   <si>
@@ -275,12 +254,6 @@
     <t>-33.40544</t>
   </si>
   <si>
-    <t>-70.55225937723938</t>
-  </si>
-  <si>
-    <t>-33.42539317947069</t>
-  </si>
-  <si>
     <t>-70.639512099</t>
   </si>
   <si>
@@ -293,18 +266,6 @@
     <t>-33.444357051398</t>
   </si>
   <si>
-    <t>-70.60831076966647</t>
-  </si>
-  <si>
-    <t>-33.43829403073846</t>
-  </si>
-  <si>
-    <t>-70.70340038</t>
-  </si>
-  <si>
-    <t>-33.5917831</t>
-  </si>
-  <si>
     <t>-70.740805595</t>
   </si>
   <si>
@@ -347,12 +308,6 @@
     <t>-33.45349244</t>
   </si>
   <si>
-    <t>-70.7598825917108</t>
-  </si>
-  <si>
-    <t>-33.5102133708451</t>
-  </si>
-  <si>
     <t>-70.6049706416048</t>
   </si>
   <si>
@@ -375,9 +330,6 @@
   </si>
   <si>
     <t>CERRILLOS</t>
-  </si>
-  <si>
-    <t>Lun a Sab 08:00 a 21:00 Dom y Festivos 09:00 a 14:00</t>
   </si>
   <si>
     <t>-70.6454652660867</t>
@@ -1007,7 +959,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:S38"/>
+  <dimension ref="A2:S34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -1124,7 +1076,7 @@
         <v>9</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="F15" s="9">
         <v>352564</v>
@@ -1133,10 +1085,10 @@
         <v>6286262</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="12" x14ac:dyDescent="0.2">
@@ -1153,7 +1105,7 @@
         <v>6</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="F16" s="9">
         <v>347803</v>
@@ -1162,10 +1114,10 @@
         <v>6306036</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="12" x14ac:dyDescent="0.2">
@@ -1182,7 +1134,7 @@
         <v>14</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="F17" s="9">
         <v>343185</v>
@@ -1191,10 +1143,10 @@
         <v>6306004</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="12" x14ac:dyDescent="0.2">
@@ -1205,13 +1157,13 @@
         <v>46</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="F18" s="9">
         <v>351432</v>
@@ -1220,10 +1172,10 @@
         <v>6293259</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="12" x14ac:dyDescent="0.2">
@@ -1240,7 +1192,7 @@
         <v>18</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="F19" s="9">
         <v>341609</v>
@@ -1249,339 +1201,359 @@
         <v>6302502</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A20" s="10">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="F20" s="9">
-        <v>355739</v>
+        <v>347788</v>
       </c>
       <c r="G20" s="9">
-        <v>6300507</v>
+        <v>6291309</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A21" s="10">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>46</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="F21" s="9">
-        <v>347788</v>
+        <v>337199</v>
       </c>
       <c r="G21" s="9">
-        <v>6291309</v>
+        <v>6298107</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>46</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="F22" s="9">
-        <v>337199</v>
+        <v>340246</v>
       </c>
       <c r="G22" s="9">
-        <v>6298107</v>
+        <v>6299652</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A23" s="10">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="F23" s="9">
-        <v>350549</v>
+        <v>347137</v>
       </c>
       <c r="G23" s="9">
-        <v>6298998</v>
+        <v>6296695</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A24" s="10">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="F24" s="9">
-        <v>341989</v>
+        <v>341522</v>
       </c>
       <c r="G24" s="9">
-        <v>6281837</v>
+        <v>6295906</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
+        <v>87</v>
+      </c>
     </row>
     <row r="25" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
+        <v>64</v>
+      </c>
+      <c r="B25" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="18" t="s">
-        <v>46</v>
-      </c>
       <c r="C25" s="9" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="F25" s="9">
-        <v>340246</v>
+        <v>348432</v>
       </c>
       <c r="G25" s="9">
-        <v>6299652</v>
+        <v>6302977</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A26" s="10">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>49</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="F26" s="9">
-        <v>347137</v>
+        <v>345636</v>
       </c>
       <c r="G26" s="9">
-        <v>6296695</v>
+        <v>6302389</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" ht="12" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A27" s="10">
-        <v>59</v>
-      </c>
-      <c r="B27" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>115</v>
+      <c r="C27" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>100</v>
       </c>
       <c r="F27" s="9">
-        <v>341522</v>
+        <v>340044</v>
       </c>
       <c r="G27" s="9">
-        <v>6295906</v>
+        <v>6292857</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" ht="12" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+    </row>
+    <row r="28" spans="1:19" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A28" s="10">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B28" s="18" t="s">
         <v>49</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="F28" s="9">
-        <v>348432</v>
+        <v>344292</v>
       </c>
       <c r="G28" s="9">
-        <v>6302977</v>
+        <v>6292613</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" ht="12" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+    </row>
+    <row r="29" spans="1:19" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A29" s="10">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="B29" s="18" t="s">
         <v>49</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="F29" s="9">
-        <v>345636</v>
+        <v>347030</v>
       </c>
       <c r="G29" s="9">
-        <v>6302389</v>
+        <v>6297244</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>104</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
     </row>
     <row r="30" spans="1:19" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A30" s="10">
-        <v>71</v>
-      </c>
-      <c r="B30" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>115</v>
+      <c r="C30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>100</v>
       </c>
       <c r="F30" s="9">
-        <v>340044</v>
+        <v>342600</v>
       </c>
       <c r="G30" s="9">
-        <v>6292857</v>
+        <v>6293992</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
@@ -1594,266 +1566,120 @@
       <c r="R30" s="2"/>
       <c r="S30" s="2"/>
     </row>
-    <row r="31" spans="1:19" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A31" s="10">
-        <v>78</v>
+    <row r="31" spans="1:19" ht="12" x14ac:dyDescent="0.2">
+      <c r="A31" s="13">
+        <v>95</v>
       </c>
       <c r="B31" s="18" t="s">
         <v>49</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="F31" s="9">
-        <v>344292</v>
+        <v>350933</v>
       </c>
       <c r="G31" s="9">
-        <v>6292613</v>
+        <v>6296934</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
-    </row>
-    <row r="32" spans="1:19" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="12" x14ac:dyDescent="0.2">
       <c r="A32" s="10">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="B32" s="18" t="s">
         <v>49</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="F32" s="9">
-        <v>347030</v>
+        <v>356883</v>
       </c>
       <c r="G32" s="9">
-        <v>6297244</v>
+        <v>6297649</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
-      <c r="Q32" s="2"/>
-      <c r="R32" s="2"/>
-      <c r="S32" s="2"/>
-    </row>
-    <row r="33" spans="1:19" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="12" x14ac:dyDescent="0.2">
       <c r="A33" s="10">
-        <v>90</v>
+        <v>113</v>
       </c>
       <c r="B33" s="18" t="s">
         <v>49</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>118</v>
+        <v>59</v>
       </c>
       <c r="E33" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F33" s="9">
+        <v>351539</v>
+      </c>
+      <c r="G33" s="9">
+        <v>6296091</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="12" x14ac:dyDescent="0.2">
+      <c r="A34" s="10">
         <v>115</v>
       </c>
-      <c r="F33" s="9">
-        <v>342600</v>
-      </c>
-      <c r="G33" s="9">
-        <v>6293992</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-      <c r="Q33" s="2"/>
-      <c r="R33" s="2"/>
-      <c r="S33" s="2"/>
-    </row>
-    <row r="34" spans="1:19" ht="12" x14ac:dyDescent="0.2">
-      <c r="A34" s="10">
-        <v>93</v>
-      </c>
-      <c r="B34" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>119</v>
+      <c r="B34" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>100</v>
       </c>
       <c r="F34" s="9">
-        <v>336593</v>
+        <v>348055</v>
       </c>
       <c r="G34" s="9">
-        <v>6290794</v>
+        <v>6299353</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" ht="12" x14ac:dyDescent="0.2">
-      <c r="A35" s="13">
-        <v>95</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F35" s="9">
-        <v>350933</v>
-      </c>
-      <c r="G35" s="9">
-        <v>6296934</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="I35" s="9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" ht="12" x14ac:dyDescent="0.2">
-      <c r="A36" s="10">
-        <v>98</v>
-      </c>
-      <c r="B36" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F36" s="9">
-        <v>356883</v>
-      </c>
-      <c r="G36" s="9">
-        <v>6297649</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" ht="12" x14ac:dyDescent="0.2">
-      <c r="A37" s="10">
-        <v>113</v>
-      </c>
-      <c r="B37" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F37" s="9">
-        <v>351539</v>
-      </c>
-      <c r="G37" s="9">
-        <v>6296091</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="I37" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" ht="12" x14ac:dyDescent="0.2">
-      <c r="A38" s="10">
-        <v>115</v>
-      </c>
-      <c r="B38" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F38" s="9">
-        <v>348055</v>
-      </c>
-      <c r="G38" s="9">
-        <v>6299353</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="I38" s="9" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1943,7 +1769,7 @@
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1980,13 +1806,13 @@
         <v>46</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="F15" s="9">
         <v>339123</v>
@@ -1995,10 +1821,10 @@
         <v>6306982</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -2015,7 +1841,7 @@
         <v>10</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="F16" s="15">
         <v>347803</v>
@@ -2024,10 +1850,10 @@
         <v>6306036</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="12" x14ac:dyDescent="0.2">
@@ -2044,7 +1870,7 @@
         <v>12</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="F17" s="9">
         <v>348592</v>
@@ -2053,10 +1879,10 @@
         <v>6286067</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -2073,7 +1899,7 @@
         <v>17</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="F18" s="15">
         <v>342431</v>
@@ -2082,10 +1908,10 @@
         <v>6289583</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="17" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -2102,7 +1928,7 @@
         <v>7</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="F19" s="15">
         <v>338267</v>
@@ -2111,10 +1937,10 @@
         <v>6294537</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>